<commit_message>
add new | add new admin page && minor tweak | minor tweak when create machine or excel import select categories in data
</commit_message>
<xml_diff>
--- a/frontend/public/Mau_Excel_MayMoc.xlsx
+++ b/frontend/public/Mau_Excel_MayMoc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin web\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\react\TPM\frontend\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62363199-BB04-4FEF-8B96-78FA20A1D262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1335EFBA-9C34-4132-BDB2-79D34997C162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,9 +55,6 @@
     <t>Ghi chú</t>
   </si>
   <si>
-    <t>Loại (Máy móc thiết bị/Phụ kiện)</t>
-  </si>
-  <si>
     <t>MAY-MAU-001</t>
   </si>
   <si>
@@ -110,13 +107,20 @@
   </si>
   <si>
     <t>Phụ kiện</t>
+  </si>
+  <si>
+    <t>Phân loại (Máy móc thiết bị/Phụ kiện)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -133,6 +137,10 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="4">
@@ -177,10 +185,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -191,8 +200,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -532,9 +543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -544,12 +553,12 @@
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="35.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -587,94 +596,94 @@
         <v>10</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="4">
+        <v>150000000</v>
+      </c>
+      <c r="H2" t="s">
         <v>17</v>
-      </c>
-      <c r="G2">
-        <v>150000000</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
       </c>
       <c r="I2">
         <v>10</v>
       </c>
-      <c r="J2">
-        <v>0</v>
+      <c r="J2" s="4">
+        <v>150000000</v>
       </c>
       <c r="K2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" t="s">
         <v>19</v>
-      </c>
-      <c r="L2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>24</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>25</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" s="4">
+        <v>5000000</v>
+      </c>
+      <c r="H3" t="s">
         <v>26</v>
-      </c>
-      <c r="G3">
-        <v>5000000</v>
-      </c>
-      <c r="H3" t="s">
-        <v>27</v>
       </c>
       <c r="I3">
         <v>5</v>
       </c>
-      <c r="J3">
-        <v>0</v>
+      <c r="J3" s="4">
+        <v>5000000</v>
       </c>
       <c r="K3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" t="s">
         <v>28</v>
-      </c>
-      <c r="L3" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576" xr:uid="{39527A25-76D3-4505-9503-2EBE09A371FA}">
       <formula1>"Máy móc thiết bị,Phụ kiện"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:K3" numberStoredAsText="1"/>
+    <ignoredError sqref="B1:K1 A3:I3 A2:I2 K2 K3" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add new | add new matrix status of machine, add new column NFC into tb_machine && remake | remake whole new approval flow
</commit_message>
<xml_diff>
--- a/frontend/public/Mau_Excel_MayMoc.xlsx
+++ b/frontend/public/Mau_Excel_MayMoc.xlsx
@@ -8,19 +8,77 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\react\TPM\frontend\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1335EFBA-9C34-4132-BDB2-79D34997C162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3095A7DB-E5C4-4D89-841B-AB7F11ADCD88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DanhSachMayMoc" sheetId="1" r:id="rId1"/>
+    <sheet name="LoaiMayMoc" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>admin</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{6C68334C-AC4E-488E-8E5E-5F07BEACB334}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">mã máy sẽ dùng công thức đánh số thứ tự dựa vào hãng sản xuất </t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="181">
   <si>
     <t>Mã máy</t>
   </si>
@@ -55,15 +113,9 @@
     <t>Ghi chú</t>
   </si>
   <si>
-    <t>MAY-MAU-001</t>
-  </si>
-  <si>
     <t>SERIAL-MAU-001</t>
   </si>
   <si>
-    <t>Máy phay CNC</t>
-  </si>
-  <si>
     <t>Model-XYZ-123</t>
   </si>
   <si>
@@ -82,15 +134,9 @@
     <t>Máy móc thiết bị</t>
   </si>
   <si>
-    <t>PK-MAU-002</t>
-  </si>
-  <si>
     <t>SERIAL-MAU-002</t>
   </si>
   <si>
-    <t>Đầu kẹp dao</t>
-  </si>
-  <si>
     <t>Model-PK-456</t>
   </si>
   <si>
@@ -106,10 +152,475 @@
     <t>Ghi chú cho phụ kiện mẫu 2</t>
   </si>
   <si>
-    <t>Phụ kiện</t>
-  </si>
-  <si>
     <t>Phân loại (Máy móc thiết bị/Phụ kiện)</t>
+  </si>
+  <si>
+    <t>NFC</t>
+  </si>
+  <si>
+    <t>NFC-12345</t>
+  </si>
+  <si>
+    <t>NFC-67890</t>
+  </si>
+  <si>
+    <t>Bàn hút</t>
+  </si>
+  <si>
+    <t>Xe nâng điện 2.5 Tấn - MGA-EF-2.5T</t>
+  </si>
+  <si>
+    <t>BAN HUT CHAN KHONG NAOMOTO FBA-Y-6512</t>
+  </si>
+  <si>
+    <t>BO DIEU TIET THUN</t>
+  </si>
+  <si>
+    <t>BO TRO LUC 1 KIM</t>
+  </si>
+  <si>
+    <t>BO TRO LUC 1 KIM DDL-9000B</t>
+  </si>
+  <si>
+    <t>BO TRO LUC 1 KIM DDL-9000C/AK154</t>
+  </si>
+  <si>
+    <t>BO TRO LUC 1 KIM PL-5515/DDL-9000B</t>
+  </si>
+  <si>
+    <t>BO TRO LUC 2 KIM</t>
+  </si>
+  <si>
+    <t>BO TRO LUC CUON SUON</t>
+  </si>
+  <si>
+    <t>BO TRO LUC MAY 1 KIM</t>
+  </si>
+  <si>
+    <t>BO TRO LUC VAT SO</t>
+  </si>
+  <si>
+    <t>BO XA DAY VIEN RACING</t>
+  </si>
+  <si>
+    <t>Chuyền hanger</t>
+  </si>
+  <si>
+    <t>Máy  KANSAI</t>
+  </si>
+  <si>
+    <t>Máy  Kansai 12K</t>
+  </si>
+  <si>
+    <t>MAY 01 KIM CO DAO XEN VAI JUKI DLM-5200NF(3/16\"\")W/MOTOR HENZ RS-03-55</t>
+  </si>
+  <si>
+    <t>Máy 1 kim</t>
+  </si>
+  <si>
+    <t>MAY 1 KIM DAU TUM</t>
+  </si>
+  <si>
+    <t>MAY 1 KIM DIEN TU JUKI DDL-9000B MS WBK/CP-180A</t>
+  </si>
+  <si>
+    <t>MAY 1 KIM DIEN TU JUKI DDL-9000CFMS-NB/SC950AK</t>
+  </si>
+  <si>
+    <t>Máy 1 kim đế ống</t>
+  </si>
+  <si>
+    <t>Máy 1 kim điện tử  JUKI DDL-9000CFMS-NB/SC950AK</t>
+  </si>
+  <si>
+    <t>May 1 kim điện tử JUKI DDL-9000CFMS-NB/SC950AK</t>
+  </si>
+  <si>
+    <t>May 1 kim điện tử JUKIDDL-9000CFMS-NB/SC950AK</t>
+  </si>
+  <si>
+    <t>MAY 1 KIM MAY DAP TU DONG</t>
+  </si>
+  <si>
+    <t>MAY 1 KIM MAY RAP</t>
+  </si>
+  <si>
+    <t>Máy 1 kim móc xích</t>
+  </si>
+  <si>
+    <t>Máy 1 kim xén</t>
+  </si>
+  <si>
+    <t>MAY 1 KIM XEN DIEN TU</t>
+  </si>
+  <si>
+    <t>MAY 1 KIM XEN JACK</t>
+  </si>
+  <si>
+    <t>MAY 1KIM DAU TUM</t>
+  </si>
+  <si>
+    <t>Máy 2 kim</t>
+  </si>
+  <si>
+    <t>MAY 2 KIM CAT CHI TU DONG</t>
+  </si>
+  <si>
+    <t>MAY 2 KIM DI DONG BROTHER T8450C-003 W/MOTOR HENZ-03-550</t>
+  </si>
+  <si>
+    <t>MAY 2 KIM DI DONG XEN CUON VIEN 1/4''</t>
+  </si>
+  <si>
+    <t>Máy 2 kim móc xích</t>
+  </si>
+  <si>
+    <t>MAY CAT GOC - LON CO AO</t>
+  </si>
+  <si>
+    <t>MAY CAT NOI THUN TU DONG - SIV</t>
+  </si>
+  <si>
+    <t>MAY CAT TAY KM KS-AUV 10''</t>
+  </si>
+  <si>
+    <t>MAY CAT TAY KM KS-AUV 13''</t>
+  </si>
+  <si>
+    <t>MAY CAT TAY KM KS-AUV 5''</t>
+  </si>
+  <si>
+    <t>MAY CAT TAY KM KS-AUV 8''</t>
+  </si>
+  <si>
+    <t>MAY CAT TAY KSM-9003 15''</t>
+  </si>
+  <si>
+    <t>Máy cắt dây nhám</t>
+  </si>
+  <si>
+    <t>Máy cắt nhãn</t>
+  </si>
+  <si>
+    <t>Máy cắt rập</t>
+  </si>
+  <si>
+    <t>Máy cắt vải tự động</t>
+  </si>
+  <si>
+    <t>MAY CUON SUON JUKI MS-1190</t>
+  </si>
+  <si>
+    <t>Máy cuốn sườn 2 kim</t>
+  </si>
+  <si>
+    <t>MAY DAN NHAN UPC</t>
+  </si>
+  <si>
+    <t>MAY DANH BONG CAT CHI TU DONG W1562P-01Gx356BS/UT4/WS-658X-STRONG H</t>
+  </si>
+  <si>
+    <t>MAY DANH BONG DAU NHO PEGASUS W264HP-01GB-356</t>
+  </si>
+  <si>
+    <t>MAY DANH BONG PEGASUS W562PV-01G-364BS  W/ MOTUER HENZ RS-03-750</t>
+  </si>
+  <si>
+    <t>MAY DANH BONG PEGASUS W662-01GX356BS W/MOTOR HENZ RS-03-500</t>
+  </si>
+  <si>
+    <t>MAY DAP NUT HOI JINLING JLQ-01-100SH</t>
+  </si>
+  <si>
+    <t>MAY DAP NUT HOI JINLING JLQ-01-125SH</t>
+  </si>
+  <si>
+    <t>Máy dập cố định TEX 4060</t>
+  </si>
+  <si>
+    <t>Máy dò kim dạng băng tải</t>
+  </si>
+  <si>
+    <t>Máy đánh bông 3 kim</t>
+  </si>
+  <si>
+    <t>Máy đánh bông 4 kim cùi chỏ</t>
+  </si>
+  <si>
+    <t>Máy đánh bông đầu nhỏ</t>
+  </si>
+  <si>
+    <t>Máy đánh số trên vải tự động</t>
+  </si>
+  <si>
+    <t>Máy đính bọ</t>
+  </si>
+  <si>
+    <t>Máy đính nút</t>
+  </si>
+  <si>
+    <t>Máy ép keo</t>
+  </si>
+  <si>
+    <t>MAY EP KEO  KANNEGIESSER</t>
+  </si>
+  <si>
+    <t>MAY EP NHAN DAU TRUOT TEXENCO</t>
+  </si>
+  <si>
+    <t>MAY EP NHAN KHO NHO H&amp;H</t>
+  </si>
+  <si>
+    <t>MAY EP NHAN MAM DOI H&amp;H CS685</t>
+  </si>
+  <si>
+    <t>MAY EP NHAN MAM TRUOT TEXENCO</t>
+  </si>
+  <si>
+    <t>Máy ép nhiệt</t>
+  </si>
+  <si>
+    <t>Máy gá túi và may tự động</t>
+  </si>
+  <si>
+    <t>Máy gá túi và may tự động NF-M320-V2.0 ( không bao gồm đầu máy may)</t>
+  </si>
+  <si>
+    <t>Máy gấp đôi và ủi nhãn 3 đầu</t>
+  </si>
+  <si>
+    <t>Máy hút ẩm công nghiệp</t>
+  </si>
+  <si>
+    <t>Máy hút chỉ 7.5Hp</t>
+  </si>
+  <si>
+    <t>Máy kiểm vải đa năng</t>
+  </si>
+  <si>
+    <t>MAY LAP TRINH BROTHER BAS-326HN W/PROGRAMER</t>
+  </si>
+  <si>
+    <t>MAY LAP TRINH HOSHIMA</t>
+  </si>
+  <si>
+    <t>MAY LAP TRINH KHO NHO</t>
+  </si>
+  <si>
+    <t>MAY LAP TRINH ZOJE KHO LON</t>
+  </si>
+  <si>
+    <t>Máy lập trình</t>
+  </si>
+  <si>
+    <t>Máy lộn ống quần - 138</t>
+  </si>
+  <si>
+    <t>Máy lượt nhãn tự động</t>
+  </si>
+  <si>
+    <t>Máy may 1 kim xén cắt chỉ tự động</t>
+  </si>
+  <si>
+    <t>Máy may 1 kim xén JK-5559F-W</t>
+  </si>
+  <si>
+    <t>Máy may bo 2 kim</t>
+  </si>
+  <si>
+    <t>Máy may bo tay 1 kim</t>
+  </si>
+  <si>
+    <t>Máy may bo tay 2 kim</t>
+  </si>
+  <si>
+    <t>Máy may chương trình</t>
+  </si>
+  <si>
+    <t>Máy may công nghiệp</t>
+  </si>
+  <si>
+    <t>Máy may công nghiệp 02 kim cơ động ổ nhỏ - Hikari - HT9220TC-7P-5/AK</t>
+  </si>
+  <si>
+    <t>Máy may công nghiệp 1 kim cổ nhỏ GTG-4251CPB</t>
+  </si>
+  <si>
+    <t>Máy may công nghiệp lập trình điện tử khổ nhỏ đế bằng</t>
+  </si>
+  <si>
+    <t>Máy may công nghiệp tự động</t>
+  </si>
+  <si>
+    <t>Máy may đáp túi tự động</t>
+  </si>
+  <si>
+    <t>Máy may đáp tự động</t>
+  </si>
+  <si>
+    <t>Máy may lập trình dùng cho ngành may CN - GTG - GT-10060-HL-QX</t>
+  </si>
+  <si>
+    <t>Máy may lập trình GTG</t>
+  </si>
+  <si>
+    <t>Máy may lập trình khổ nhỏ, dùng cho ngành may CN - GTG - GT- 1906</t>
+  </si>
+  <si>
+    <t>Máy may lập trình thông minh BOK-S80-40-HL</t>
+  </si>
+  <si>
+    <t>Máy may lập trình thông minh( có laser) BOK-S80-40-HL-JG</t>
+  </si>
+  <si>
+    <t>Máy may miệng túi</t>
+  </si>
+  <si>
+    <t>Máy may nhãn tự động</t>
+  </si>
+  <si>
+    <t>Máy may nhãn tự động LENSH LS-8121</t>
+  </si>
+  <si>
+    <t>Máy may trang trí điện tử</t>
+  </si>
+  <si>
+    <t>Máy may viền xén trái điện tử</t>
+  </si>
+  <si>
+    <t>MAY MIENG TUI TU DONG</t>
+  </si>
+  <si>
+    <t>Máy mổ túi JUKI APW</t>
+  </si>
+  <si>
+    <t>Máy nén khí trục vít có dầu, biến tần</t>
+  </si>
+  <si>
+    <t>Máy nén khí trục vít có dầu, tố độ cố định</t>
+  </si>
+  <si>
+    <t>Máy nối thun</t>
+  </si>
+  <si>
+    <t>Máy phát điện</t>
+  </si>
+  <si>
+    <t>MAY PHAY RAP MICCA TU DONG</t>
+  </si>
+  <si>
+    <t>Máy quấn chân nút cắt chỉ tự động A708 - ISN</t>
+  </si>
+  <si>
+    <t>Máy sấy khô khí nén</t>
+  </si>
+  <si>
+    <t>MAY THUA  KHUY TRON</t>
+  </si>
+  <si>
+    <t>Máy thùa khuy</t>
+  </si>
+  <si>
+    <t>MAY THUA KHUY DAU TRON HIKARI</t>
+  </si>
+  <si>
+    <t>MAY THUA KHUY DIEN TU JUKI LBH-1790AN</t>
+  </si>
+  <si>
+    <t>MAY THUA KHUY DIEN TU JUKI MEB-3200 CSSKA (Dong bo)</t>
+  </si>
+  <si>
+    <t>MAY THUA KHUY DIEN TU TU DONG - SIV</t>
+  </si>
+  <si>
+    <t>MAY THUA KHUY DOI TU DONG</t>
+  </si>
+  <si>
+    <t>MAY THUA KHUY DT JUKI LBH-1790AS/MC602KS</t>
+  </si>
+  <si>
+    <t>Máy thùa khuy điện tử JUKI LBH-1790ANS/MC602KN</t>
+  </si>
+  <si>
+    <t>Máy thùa tròn</t>
+  </si>
+  <si>
+    <t>Máy trải vải tự động</t>
+  </si>
+  <si>
+    <t>MAY VAT SO 5 CHI JUKI MO-6816 DDE4-30H-AA1/ SV82</t>
+  </si>
+  <si>
+    <t>MAY VAT SO 5 CHI MO-6816-DDE4-30H-?35/W MOTOR HENZ RS-03-988</t>
+  </si>
+  <si>
+    <t>MAY VAT SO DAU TUM  PEGASUS EX5114-03/333N-2X4/PT</t>
+  </si>
+  <si>
+    <t>MAY VAT SO JUKI MO-6816D-1D6-40H W/MOTOR ISEWIS-JN 6816-5ETK</t>
+  </si>
+  <si>
+    <t>MAY VAT SO JUKI MO-6843D-1D6-40H W/MOTOR ISM SV-82 DD-CONVERSION PART</t>
+  </si>
+  <si>
+    <t>MAY VAT SO MO-6816D-DE4-30H W/MOTOR HENZ MO-6800-ETK ( CAT CHI TU DONG )</t>
+  </si>
+  <si>
+    <t>MAY VE CAT RAP GIAY TU DONG</t>
+  </si>
+  <si>
+    <t>MAY VE SO DO FASTJET PRO-2203</t>
+  </si>
+  <si>
+    <t>Máy vẽ sơ đồ</t>
+  </si>
+  <si>
+    <t>Máy VS</t>
+  </si>
+  <si>
+    <t>Máy VS 2K</t>
+  </si>
+  <si>
+    <t>Máy VS 2K4C</t>
+  </si>
+  <si>
+    <t>Máy VS 2K5C</t>
+  </si>
+  <si>
+    <t>Máy VS 3K6C</t>
+  </si>
+  <si>
+    <t>MAY XEN 1 KIM DIEN TU</t>
+  </si>
+  <si>
+    <t>Máy zigzag</t>
+  </si>
+  <si>
+    <t>Máy zigzag 1K</t>
+  </si>
+  <si>
+    <t>NOI HOI DIEN 18 KW TEXENCO</t>
+  </si>
+  <si>
+    <t>NOI HOI DIEN 9 KW TEXENCO</t>
+  </si>
+  <si>
+    <t>Nồi hơi 6KW</t>
+  </si>
+  <si>
+    <t>Nồi hơi Texenco 18KW</t>
+  </si>
+  <si>
+    <t>Nồi hơi Texenco 9KW</t>
+  </si>
+  <si>
+    <t>Thiết bị chuyển hướng máy dò kim</t>
+  </si>
+  <si>
+    <t>Xe nâng điện 1.5 Tấn - MGA-ESH-45</t>
+  </si>
+  <si>
+    <t>Xe nâng điện 1.5 Tấn - MGA-ESH-45 (XN2)</t>
   </si>
 </sst>
 </file>
@@ -118,9 +629,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -141,6 +652,13 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -200,7 +718,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -540,28 +1058,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -581,109 +1103,915 @@
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="M1" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="str" cm="1">
+        <f t="array" ref="A2">SUBSTITUTE(E2," ","") &amp;
+TEXT(SUMPRODUCT(--(SUBSTITUTE($E$2:E2," ","") = SUBSTITUTE(E2," ",""))), "00000")</f>
+        <v>HãngSXA00001</v>
+      </c>
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="4">
+        <v>150000000</v>
+      </c>
+      <c r="I2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s">
+      <c r="J2">
+        <v>10</v>
+      </c>
+      <c r="K2" s="4">
+        <v>150000000</v>
+      </c>
+      <c r="L2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="4">
-        <v>150000000</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="M2" t="s">
         <v>17</v>
       </c>
-      <c r="I2">
-        <v>10</v>
-      </c>
-      <c r="J2" s="4">
-        <v>150000000</v>
-      </c>
-      <c r="K2" t="s">
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="str" cm="1">
+        <f t="array" ref="A3">SUBSTITUTE(E3," ","") &amp;
+TEXT(SUMPRODUCT(--(SUBSTITUTE($E$2:E3," ","") = SUBSTITUTE(E3," ",""))), "00000")</f>
+        <v>HãngSXB00001</v>
+      </c>
+      <c r="B3" t="s">
         <v>18</v>
       </c>
-      <c r="L2" t="s">
+      <c r="D3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="E3" t="s">
         <v>20</v>
       </c>
-      <c r="B3" t="s">
+      <c r="F3" t="s">
         <v>21</v>
       </c>
-      <c r="C3" t="s">
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="4">
+        <v>5000000</v>
+      </c>
+      <c r="I3" t="s">
         <v>22</v>
       </c>
-      <c r="D3" t="s">
+      <c r="J3">
+        <v>5</v>
+      </c>
+      <c r="K3" s="4">
+        <v>5000000</v>
+      </c>
+      <c r="L3" t="s">
         <v>23</v>
       </c>
-      <c r="E3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="4">
-        <v>5000000</v>
-      </c>
-      <c r="H3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3">
-        <v>5</v>
-      </c>
-      <c r="J3" s="4">
-        <v>5000000</v>
-      </c>
-      <c r="K3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L3" t="s">
-        <v>28</v>
+      <c r="M3" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576" xr:uid="{39527A25-76D3-4505-9503-2EBE09A371FA}">
-      <formula1>"Máy móc thiết bị,Phụ kiện"</formula1>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M1048576" xr:uid="{9F268F74-316A-4C1A-BE8C-AAD87BA65D3F}">
+      <formula1>"Máy móc thiết bị"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="B1:K1 A3:I3 A2:I2 K2 K3" numberStoredAsText="1"/>
+    <ignoredError sqref="H1:L1 H2:J3 L2:L3 B3 B1:F1 B2 D3:F3 D2:F2" numberStoredAsText="1"/>
   </ignoredErrors>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A235E470-EFC7-49E0-B06E-31C3A85CD3FF}">
+          <x14:formula1>
+            <xm:f>LoaiMayMoc!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{983E5464-CEE9-41EE-8EED-83216360782C}">
+  <dimension ref="A1:A153"/>
+  <sheetViews>
+    <sheetView topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="A150" sqref="A150"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="82.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1">
+      <c r="A139" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1">
+      <c r="A140" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1">
+      <c r="A141" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1">
+      <c r="A142" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1">
+      <c r="A143" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1">
+      <c r="A144" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1">
+      <c r="A145" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1">
+      <c r="A146" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1">
+      <c r="A147" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1">
+      <c r="A148" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1">
+      <c r="A149" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1">
+      <c r="A150" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1">
+      <c r="A151" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1">
+      <c r="A153" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
minor tweak | minor tweak import machine list via excel
</commit_message>
<xml_diff>
--- a/frontend/public/Mau_Excel_MayMoc.xlsx
+++ b/frontend/public/Mau_Excel_MayMoc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\react\TPM\frontend\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3095A7DB-E5C4-4D89-841B-AB7F11ADCD88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9C32CF-FBE0-456C-BE3E-C7443D4F2A69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DanhSachMayMoc" sheetId="1" r:id="rId1"/>
@@ -31,57 +31,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>admin</author>
-  </authors>
-  <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{6C68334C-AC4E-488E-8E5E-5F07BEACB334}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">mã máy sẽ dùng công thức đánh số thứ tự dựa vào hãng sản xuất </t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="181">
-  <si>
-    <t>Mã máy</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="177">
   <si>
     <t>Serial</t>
   </si>
@@ -119,9 +70,6 @@
     <t>Model-XYZ-123</t>
   </si>
   <si>
-    <t>Hãng SX A</t>
-  </si>
-  <si>
     <t>RFID-12345</t>
   </si>
   <si>
@@ -131,18 +79,12 @@
     <t>Ghi chú cho máy mẫu 1</t>
   </si>
   <si>
-    <t>Máy móc thiết bị</t>
-  </si>
-  <si>
     <t>SERIAL-MAU-002</t>
   </si>
   <si>
     <t>Model-PK-456</t>
   </si>
   <si>
-    <t>Hãng SX B</t>
-  </si>
-  <si>
     <t>RFID-67890</t>
   </si>
   <si>
@@ -152,9 +94,6 @@
     <t>Ghi chú cho phụ kiện mẫu 2</t>
   </si>
   <si>
-    <t>Phân loại (Máy móc thiết bị/Phụ kiện)</t>
-  </si>
-  <si>
     <t>NFC</t>
   </si>
   <si>
@@ -621,6 +560,9 @@
   </si>
   <si>
     <t>Xe nâng điện 1.5 Tấn - MGA-ESH-45 (XN2)</t>
+  </si>
+  <si>
+    <t>Tên hãng SX</t>
   </si>
 </sst>
 </file>
@@ -631,7 +573,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -653,25 +595,13 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -707,12 +637,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1058,166 +985,139 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" hidden="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2">SUBSTITUTE(E2," ","") &amp;
-TEXT(SUMPRODUCT(--(SUBSTITUTE($E$2:E2," ","") = SUBSTITUTE(E2," ",""))), "00000")</f>
-        <v>HãngSXA00001</v>
-      </c>
       <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
-        <v>62</v>
-      </c>
       <c r="D2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="3">
+        <v>150000000</v>
+      </c>
+      <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2">
+        <v>10</v>
+      </c>
+      <c r="J2" s="3">
+        <v>150000000</v>
+      </c>
+      <c r="K2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="4">
-        <v>150000000</v>
-      </c>
-      <c r="I2" t="s">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>15</v>
       </c>
-      <c r="J2">
-        <v>10</v>
-      </c>
-      <c r="K2" s="4">
-        <v>150000000</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="B3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="M2" t="s">
+      <c r="D3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" t="str" cm="1">
-        <f t="array" ref="A3">SUBSTITUTE(E3," ","") &amp;
-TEXT(SUMPRODUCT(--(SUBSTITUTE($E$2:E3," ","") = SUBSTITUTE(E3," ",""))), "00000")</f>
-        <v>HãngSXB00001</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="3">
+        <v>5000000</v>
+      </c>
+      <c r="H3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" t="s">
+      <c r="I3">
+        <v>5</v>
+      </c>
+      <c r="J3" s="3">
+        <v>5000000</v>
+      </c>
+      <c r="K3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" s="4">
-        <v>5000000</v>
-      </c>
-      <c r="I3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3">
-        <v>5</v>
-      </c>
-      <c r="K3" s="4">
-        <v>5000000</v>
-      </c>
-      <c r="L3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M3" t="s">
-        <v>17</v>
-      </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M1048576" xr:uid="{9F268F74-316A-4C1A-BE8C-AAD87BA65D3F}">
-      <formula1>"Máy móc thiết bị"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="H1:L1 H2:J3 L2:L3 B3 B1:F1 B2 D3:F3 D2:F2" numberStoredAsText="1"/>
+    <ignoredError sqref="G1:K1 G2:I3 K2:K3 A3 A1:E1 A2 C3 C2 E2 E3" numberStoredAsText="1"/>
   </ignoredErrors>
-  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -1225,7 +1125,7 @@
           <x14:formula1>
             <xm:f>LoaiMayMoc!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C1048576</xm:sqref>
+          <xm:sqref>B2:B1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1241,774 +1141,774 @@
       <selection activeCell="A150" sqref="A150"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="82.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
-      <c r="A12" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
-      <c r="A15" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
-      <c r="A16" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
-      <c r="A21" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
-      <c r="A22" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
-      <c r="A23" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
-      <c r="A24" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
-      <c r="A25" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
-      <c r="A26" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
-      <c r="A27" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
-      <c r="A28" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
-      <c r="A29" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
-      <c r="A30" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
-      <c r="A31" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
-      <c r="A32" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
-      <c r="A33" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
-      <c r="A34" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
-      <c r="A35" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
-      <c r="A36" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
-      <c r="A37" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
-      <c r="A38" t="s">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
-      <c r="A39" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
-      <c r="A40" t="s">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
-      <c r="A41" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
-      <c r="A42" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
-      <c r="A43" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
-      <c r="A44" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
-      <c r="A45" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
-      <c r="A46" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
-      <c r="A47" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
-      <c r="A48" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
-      <c r="A49" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
-      <c r="A50" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
-      <c r="A51" t="s">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
-      <c r="A52" t="s">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
-      <c r="A53" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
-      <c r="A54" t="s">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
-      <c r="A55" t="s">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
-      <c r="A56" t="s">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
-      <c r="A57" t="s">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
-      <c r="A58" t="s">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
-      <c r="A59" t="s">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="60" spans="1:1">
-      <c r="A60" t="s">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
-      <c r="A61" t="s">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
-      <c r="A62" t="s">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
-      <c r="A63" t="s">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="64" spans="1:1">
-      <c r="A64" t="s">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
-      <c r="A65" t="s">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
-      <c r="A66" t="s">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="67" spans="1:1">
-      <c r="A67" t="s">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="68" spans="1:1">
-      <c r="A68" t="s">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="69" spans="1:1">
-      <c r="A69" t="s">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="70" spans="1:1">
-      <c r="A70" t="s">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
-      <c r="A71" t="s">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="72" spans="1:1">
-      <c r="A72" t="s">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="73" spans="1:1">
-      <c r="A73" t="s">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="74" spans="1:1">
-      <c r="A74" t="s">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="75" spans="1:1">
-      <c r="A75" t="s">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="76" spans="1:1">
-      <c r="A76" t="s">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
-      <c r="A77" t="s">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="78" spans="1:1">
-      <c r="A78" t="s">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="79" spans="1:1">
-      <c r="A79" t="s">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="80" spans="1:1">
-      <c r="A80" t="s">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="81" spans="1:1">
-      <c r="A81" t="s">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="82" spans="1:1">
-      <c r="A82" t="s">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="83" spans="1:1">
-      <c r="A83" t="s">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="84" spans="1:1">
-      <c r="A84" t="s">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="85" spans="1:1">
-      <c r="A85" t="s">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="86" spans="1:1">
-      <c r="A86" t="s">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="87" spans="1:1">
-      <c r="A87" t="s">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="88" spans="1:1">
-      <c r="A88" t="s">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="89" spans="1:1">
-      <c r="A89" t="s">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="90" spans="1:1">
-      <c r="A90" t="s">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="91" spans="1:1">
-      <c r="A91" t="s">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="92" spans="1:1">
-      <c r="A92" t="s">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="93" spans="1:1">
-      <c r="A93" t="s">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="94" spans="1:1">
-      <c r="A94" t="s">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="95" spans="1:1">
-      <c r="A95" t="s">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="96" spans="1:1">
-      <c r="A96" t="s">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="97" spans="1:1">
-      <c r="A97" t="s">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="98" spans="1:1">
-      <c r="A98" t="s">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="99" spans="1:1">
-      <c r="A99" t="s">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="100" spans="1:1">
-      <c r="A100" t="s">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="101" spans="1:1">
-      <c r="A101" t="s">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="102" spans="1:1">
-      <c r="A102" t="s">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="103" spans="1:1">
-      <c r="A103" t="s">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="104" spans="1:1">
-      <c r="A104" t="s">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="105" spans="1:1">
-      <c r="A105" t="s">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="106" spans="1:1">
-      <c r="A106" t="s">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="107" spans="1:1">
-      <c r="A107" t="s">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="108" spans="1:1">
-      <c r="A108" t="s">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="109" spans="1:1">
-      <c r="A109" t="s">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="110" spans="1:1">
-      <c r="A110" t="s">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="111" spans="1:1">
-      <c r="A111" t="s">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="112" spans="1:1">
-      <c r="A112" t="s">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="113" spans="1:1">
-      <c r="A113" t="s">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="114" spans="1:1">
-      <c r="A114" t="s">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="115" spans="1:1">
-      <c r="A115" t="s">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="116" spans="1:1">
-      <c r="A116" t="s">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="117" spans="1:1">
-      <c r="A117" t="s">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="118" spans="1:1">
-      <c r="A118" t="s">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="119" spans="1:1">
-      <c r="A119" t="s">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="120" spans="1:1">
-      <c r="A120" t="s">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="121" spans="1:1">
-      <c r="A121" t="s">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="122" spans="1:1">
-      <c r="A122" t="s">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="123" spans="1:1">
-      <c r="A123" t="s">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="124" spans="1:1">
-      <c r="A124" t="s">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="125" spans="1:1">
-      <c r="A125" t="s">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="126" spans="1:1">
-      <c r="A126" t="s">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="127" spans="1:1">
-      <c r="A127" t="s">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="128" spans="1:1">
-      <c r="A128" t="s">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="129" spans="1:1">
-      <c r="A129" t="s">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="130" spans="1:1">
-      <c r="A130" t="s">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="131" spans="1:1">
-      <c r="A131" t="s">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="132" spans="1:1">
-      <c r="A132" t="s">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="133" spans="1:1">
-      <c r="A133" t="s">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="134" spans="1:1">
-      <c r="A134" t="s">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="135" spans="1:1">
-      <c r="A135" t="s">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="136" spans="1:1">
-      <c r="A136" t="s">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="137" spans="1:1">
-      <c r="A137" t="s">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="138" spans="1:1">
-      <c r="A138" t="s">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="139" spans="1:1">
-      <c r="A139" t="s">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="140" spans="1:1">
-      <c r="A140" t="s">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="141" spans="1:1">
-      <c r="A141" t="s">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="142" spans="1:1">
-      <c r="A142" t="s">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="143" spans="1:1">
-      <c r="A143" t="s">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="144" spans="1:1">
-      <c r="A144" t="s">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="145" spans="1:1">
-      <c r="A145" t="s">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="146" spans="1:1">
-      <c r="A146" t="s">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="147" spans="1:1">
-      <c r="A147" t="s">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="148" spans="1:1">
-      <c r="A148" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="149" spans="1:1">
-      <c r="A149" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="150" spans="1:1">
-      <c r="A150" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="151" spans="1:1">
-      <c r="A151" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="152" spans="1:1">
-      <c r="A152" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="153" spans="1:1">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjust | adjust mobile UI && adjust UI for new attribute of machine
</commit_message>
<xml_diff>
--- a/frontend/public/Mau_Excel_MayMoc.xlsx
+++ b/frontend/public/Mau_Excel_MayMoc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\react\TPM\frontend\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A87F7D-FF13-462E-BD84-59D07B7608CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E98A48-0F65-4DB4-9E60-B8D520DE3C79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="DanhSachMayMoc" sheetId="1" r:id="rId1"/>
     <sheet name="LoaiMayMoc" sheetId="2" r:id="rId2"/>
     <sheet name="HangSX" sheetId="3" r:id="rId3"/>
+    <sheet name="NhaCungCap" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>Serial</t>
   </si>
@@ -111,6 +112,30 @@
   </si>
   <si>
     <t>BAOYU</t>
+  </si>
+  <si>
+    <t>Nhà cung cấp</t>
+  </si>
+  <si>
+    <t>Đặc tính</t>
+  </si>
+  <si>
+    <t>10x20</t>
+  </si>
+  <si>
+    <t>20x30</t>
+  </si>
+  <si>
+    <t>Công suất</t>
+  </si>
+  <si>
+    <t>Áp suất</t>
+  </si>
+  <si>
+    <t>Điện áp</t>
+  </si>
+  <si>
+    <t>GIANG THÀNH</t>
   </si>
 </sst>
 </file>
@@ -534,65 +559,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -600,34 +645,49 @@
         <v>23</v>
       </c>
       <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>25</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>21</v>
-      </c>
-      <c r="G2" s="3">
-        <v>150000000</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
       </c>
       <c r="I2">
         <v>10</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2">
+        <v>15</v>
+      </c>
+      <c r="K2">
+        <v>20</v>
+      </c>
+      <c r="L2" s="3">
         <v>150000000</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2">
+        <v>10</v>
+      </c>
+      <c r="O2" s="3">
+        <v>150000000</v>
+      </c>
+      <c r="P2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -635,41 +695,47 @@
         <v>24</v>
       </c>
       <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>25</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="3">
+      <c r="L3" s="3">
         <v>5000000</v>
       </c>
-      <c r="H3" t="s">
+      <c r="M3" t="s">
         <v>18</v>
       </c>
-      <c r="I3">
+      <c r="N3">
         <v>5</v>
       </c>
-      <c r="J3" s="3">
+      <c r="O3" s="3">
         <v>5000000</v>
       </c>
-      <c r="K3" t="s">
+      <c r="P3" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="G1:K1 G2:I3 K2:K3 A3 A1:E1 A2 C3 C2 E2 E3" numberStoredAsText="1"/>
+    <ignoredError sqref="L1:P1 L2:N3 P2:P3 A2:A3 D2:D3 G1:G3 D1:E1 A1:B1" numberStoredAsText="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A235E470-EFC7-49E0-B06E-31C3A85CD3FF}">
           <x14:formula1>
             <xm:f>LoaiMayMoc!$A:$A</xm:f>
@@ -680,7 +746,19 @@
           <x14:formula1>
             <xm:f>HangSX!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D1048576</xm:sqref>
+          <xm:sqref>E2:E1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{61D70CBA-93CC-45AF-85D1-5A24C6AC0E32}">
+          <x14:formula1>
+            <xm:f>NhaCungCap!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{472E5E5B-407E-4F2E-BAC6-82849E509BD9}">
+          <x14:formula1>
+            <xm:f>LoaiMayMoc!$B:$B</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -692,9 +770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{983E5464-CEE9-41EE-8EED-83216360782C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -706,9 +782,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04243702-2A7A-45A5-BBE3-5C41301554E1}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A1048557" workbookViewId="0">
-      <selection activeCell="A1048575" sqref="A1048575"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{078887F3-BA3E-484B-B931-5F112A68A033}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>